<commit_message>
add updated Master Excel as of 9-30-20
</commit_message>
<xml_diff>
--- a/scraper/Database_Master.xlsx
+++ b/scraper/Database_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iqtcloud.sharepoint.com/sites/MS-COVID-19TestingTeam/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7846" documentId="8_{E667D74E-7E7B-584B-B180-6F5CFBAA04E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24F71B9C-EBF5-4F26-AB0F-E3588C3412EE}"/>
+  <xr:revisionPtr revIDLastSave="7901" documentId="8_{E667D74E-7E7B-584B-B180-6F5CFBAA04E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26F09CF8-C5A3-44E5-9565-1007CEC0C7AD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sample Types" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combined Molec&amp;Antigen Tests'!$A$1:$AG$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combined Molec&amp;Antigen Tests'!$A$1:$AG$207</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Molecular test kits'!$A$1:$AG$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6807" uniqueCount="2389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6853" uniqueCount="2408">
   <si>
     <t>Company</t>
   </si>
@@ -7366,6 +7366,63 @@
   </si>
   <si>
     <t>nasal swab; target was human RNase P gene</t>
+  </si>
+  <si>
+    <t>Xpert Xpress SARS-CoV-2/Flu/RSV</t>
+  </si>
+  <si>
+    <t>https://www.fda.gov/media/142437/download</t>
+  </si>
+  <si>
+    <t>XPCOV2/FLU/RSV-10</t>
+  </si>
+  <si>
+    <t>46/47</t>
+  </si>
+  <si>
+    <t>193/193</t>
+  </si>
+  <si>
+    <t>data here only for SARS-CoV-2; IFU doc also contains data for flu A, flu B PPA/NPA</t>
+  </si>
+  <si>
+    <t>Clear Labs, Inc.</t>
+  </si>
+  <si>
+    <t>Clear Dx SARS-CoV-2 Test</t>
+  </si>
+  <si>
+    <t>Clear Dx™ SARS-CoV-2 Test</t>
+  </si>
+  <si>
+    <t>https://www.fda.gov/media/142418/download</t>
+  </si>
+  <si>
+    <t>https://www.clearlabs.com/covid-19/</t>
+  </si>
+  <si>
+    <t>Clear Dx, Oxford Nanopore GridION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service@clearlabs.com </t>
+  </si>
+  <si>
+    <t>1-650-257-3304</t>
+  </si>
+  <si>
+    <t>1-888-838-3222</t>
+  </si>
+  <si>
+    <t>1559 Industrial Road</t>
+  </si>
+  <si>
+    <t>San Carlos</t>
+  </si>
+  <si>
+    <t>Quadrant Biosciences Inc.</t>
+  </si>
+  <si>
+    <t>Vela Operations Singapore Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -8452,8 +8509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F543DF2C-2287-6C4A-8AF4-94B0E420CECB}" name="Table1" displayName="Table1" ref="A1:AK204" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="A1:AK204" xr:uid="{6F6113B7-EEAD-4540-921E-D13DCBA1AB47}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F543DF2C-2287-6C4A-8AF4-94B0E420CECB}" name="Table1" displayName="Table1" ref="A1:AK207" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:AK207" xr:uid="{6F6113B7-EEAD-4540-921E-D13DCBA1AB47}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK204">
     <sortCondition ref="A1:A204"/>
   </sortState>
@@ -13775,11 +13832,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8D7EB-7B57-491C-8EFF-EE7E951B406D}">
-  <dimension ref="A1:AQ204"/>
+  <dimension ref="A1:AQ207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29774,9 +29831,161 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="204" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="D204" s="5"/>
-      <c r="E204" s="5"/>
+    <row r="204" spans="1:42" ht="87" x14ac:dyDescent="0.35">
+      <c r="A204" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B204" s="23" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C204" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>2390</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F204" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G204" s="23" t="s">
+        <v>948</v>
+      </c>
+      <c r="H204" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="I204" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J204" s="23" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K204" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="L204" s="63" t="s">
+        <v>279</v>
+      </c>
+      <c r="M204" s="64" t="s">
+        <v>2403</v>
+      </c>
+      <c r="N204" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="O204" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="P204" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q204" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="R204" s="64">
+        <v>94089</v>
+      </c>
+      <c r="AK204" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="AL204" s="49" t="s">
+        <v>826</v>
+      </c>
+      <c r="AM204" s="54" t="s">
+        <v>2392</v>
+      </c>
+      <c r="AN204" s="54" t="s">
+        <v>2393</v>
+      </c>
+      <c r="AO204" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="AP204" s="49" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="205" spans="1:42" ht="58" x14ac:dyDescent="0.35">
+      <c r="A205" s="23" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B205" s="23" t="s">
+        <v>2396</v>
+      </c>
+      <c r="C205" s="23" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>2398</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>2399</v>
+      </c>
+      <c r="F205" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G205" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H205" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I205" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J205" s="23" t="s">
+        <v>2397</v>
+      </c>
+      <c r="K205" s="5" t="s">
+        <v>2401</v>
+      </c>
+      <c r="M205" s="33" t="s">
+        <v>2402</v>
+      </c>
+      <c r="N205" s="23" t="s">
+        <v>2404</v>
+      </c>
+      <c r="O205" s="23" t="s">
+        <v>2405</v>
+      </c>
+      <c r="P205" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q205" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="R205" s="23">
+        <v>94070</v>
+      </c>
+      <c r="AK205" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="AL205" s="49" t="s">
+        <v>826</v>
+      </c>
+      <c r="AM205" s="54" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AN205" s="54" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AO205" s="49" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="206" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A206" s="23" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D206" s="5"/>
+      <c r="E206" s="5"/>
+    </row>
+    <row r="207" spans="1:42" ht="29" x14ac:dyDescent="0.35">
+      <c r="A207" s="23" t="s">
+        <v>2407</v>
+      </c>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
@@ -30190,11 +30399,12 @@
     <hyperlink ref="K158" r:id="rId407" xr:uid="{51E136AE-930A-4D60-A2CE-4AD6CAD4A6EF}"/>
     <hyperlink ref="D159" r:id="rId408" xr:uid="{9A60A62A-1CB5-4420-B836-4690A5EBA8E3}"/>
     <hyperlink ref="K53" r:id="rId409" xr:uid="{61A996C7-0580-453E-BE4D-9EAC89D13E14}"/>
+    <hyperlink ref="K205" r:id="rId410" xr:uid="{229765DB-95C5-43E7-9F32-07C311B4C209}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId410"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId411"/>
   <tableParts count="1">
-    <tablePart r:id="rId411"/>
+    <tablePart r:id="rId412"/>
   </tableParts>
 </worksheet>
 </file>
@@ -34784,18 +34994,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34818,26 +35028,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FA49A7F-7C4D-4200-9628-76592D6DAB58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b04d4598-dd04-450c-aa56-46cff6b0ba6f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab860399-53f0-46d8-8140-572bffe2e624"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4480A02C-A00C-4D86-BC0D-93448CC4AD0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FA49A7F-7C4D-4200-9628-76592D6DAB58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b04d4598-dd04-450c-aa56-46cff6b0ba6f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ab860399-53f0-46d8-8140-572bffe2e624"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated master excel as of 10-29-20
</commit_message>
<xml_diff>
--- a/scraper/Database_Master.xlsx
+++ b/scraper/Database_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iqtcloud.sharepoint.com/sites/MS-COVID-19TestingTeam/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="8_{BF47ED3A-D8BD-F440-849E-0991F9D957D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A98BDEB3-AC33-A04F-9386-E38B20998385}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{BF47ED3A-D8BD-F440-849E-0991F9D957D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11086007-5079-7A43-A286-A0E893CCE95C}"/>
   <bookViews>
-    <workbookView xWindow="-34540" yWindow="-21140" windowWidth="34540" windowHeight="21140" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Molecular test kits" sheetId="13" r:id="rId1"/>
@@ -14426,8 +14426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8D7EB-7B57-491C-8EFF-EE7E951B406D}">
   <dimension ref="A1:AQ227"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AP129" sqref="AP129"/>
     </sheetView>
   </sheetViews>
@@ -34601,7 +34601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D5E236-9FEA-4257-AEA7-FAEDD9345A9C}">
   <dimension ref="A1:AH73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="S58" sqref="S58"/>
@@ -38999,21 +38999,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E670CC39FE6924EBD59906DF8EFDA53" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e90685ec06a69706c37c028f3edd6b9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b04d4598-dd04-450c-aa56-46cff6b0ba6f" xmlns:ns3="ab860399-53f0-46d8-8140-572bffe2e624" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83a6c33188c8c12d0ffda7f47847f238" ns2:_="" ns3:_="">
     <xsd:import namespace="b04d4598-dd04-450c-aa56-46cff6b0ba6f"/>
@@ -39196,32 +39181,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4480A02C-A00C-4D86-BC0D-93448CC4AD0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FA49A7F-7C4D-4200-9628-76592D6DAB58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ab860399-53f0-46d8-8140-572bffe2e624"/>
-    <ds:schemaRef ds:uri="b04d4598-dd04-450c-aa56-46cff6b0ba6f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AFB4A3B-F7DD-4E53-953B-5C63B18C09BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39238,4 +39213,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FA49A7F-7C4D-4200-9628-76592D6DAB58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b04d4598-dd04-450c-aa56-46cff6b0ba6f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ab860399-53f0-46d8-8140-572bffe2e624"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4480A02C-A00C-4D86-BC0D-93448CC4AD0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>